<commit_message>
Commit Finish Problem 1 and loading data sets for Problem 2.
</commit_message>
<xml_diff>
--- a/Problem 1/2018_Precipitation.xlsx
+++ b/Problem 1/2018_Precipitation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oliviaewagner/Documents/Columbia/First Semester/Data Science I/Homework 2/p8105_hw2_oew2106/Problem 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8A33893A-CF2E-0944-AA28-6A335B876CE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4D75136-B21B-5040-8EE7-779A435AD0AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14320" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14320" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mr. Trash Wheel" sheetId="3" r:id="rId1"/>
@@ -21562,7 +21562,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -21684,7 +21684,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>

</xml_diff>